<commit_message>
finishes butterfly pie plots
</commit_message>
<xml_diff>
--- a/allButterfly.xlsx
+++ b/allButterfly.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a1733ece3548b272/Desktop/School/GGCSpring2023/STEC/OneDrive_1_1-23-2023/Data/excelData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Desktop\School\GGCSpring2023\actualSTEC\PanoRestoration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{6E1118A9-2723-4668-8AAB-5E42E2429173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94975E52-77DE-4182-AF43-52F99CE08750}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC67D62D-31AE-456F-A273-E359D9E910D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3006" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3006" uniqueCount="337">
   <si>
     <t>Date</t>
   </si>
@@ -850,9 +850,6 @@
   </si>
   <si>
     <t>southern skipperling</t>
-  </si>
-  <si>
-    <t>fiery skipper</t>
   </si>
   <si>
     <t>crossline skipper</t>
@@ -1145,10 +1142,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1455,8 +1448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B4A887B-CF06-4E5D-8EC5-AEF2BE92881D}">
   <dimension ref="A1:F1172"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E1172"/>
+    <sheetView tabSelected="1" topLeftCell="A403" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B433" sqref="B433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1542,7 +1535,7 @@
         <v>215</v>
       </c>
       <c r="C5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E5" s="3">
         <v>17</v>
@@ -1598,7 +1591,7 @@
         <v>219</v>
       </c>
       <c r="C9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -1713,7 +1706,7 @@
         <v>246</v>
       </c>
       <c r="C17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E17" s="3">
         <v>2</v>
@@ -1783,7 +1776,7 @@
         <v>250</v>
       </c>
       <c r="C22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E22" s="3">
         <v>4</v>
@@ -1839,7 +1832,7 @@
         <v>215</v>
       </c>
       <c r="C26" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
@@ -1954,7 +1947,7 @@
         <v>246</v>
       </c>
       <c r="C34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E34" s="3">
         <v>3</v>
@@ -1982,7 +1975,7 @@
         <v>250</v>
       </c>
       <c r="C36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E36" s="3">
         <v>2</v>
@@ -2108,7 +2101,7 @@
         <v>225</v>
       </c>
       <c r="C45" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E45" s="3">
         <v>2</v>
@@ -2150,7 +2143,7 @@
         <v>221</v>
       </c>
       <c r="C48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E48" s="3">
         <v>70</v>
@@ -2184,7 +2177,7 @@
         <v>230</v>
       </c>
       <c r="C50" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E50" s="3">
         <v>11</v>
@@ -2198,7 +2191,7 @@
         <v>231</v>
       </c>
       <c r="C51" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E51" s="3">
         <v>2</v>
@@ -2322,7 +2315,7 @@
         <v>246</v>
       </c>
       <c r="C59" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E59" s="3">
         <v>3</v>
@@ -2364,7 +2357,7 @@
         <v>250</v>
       </c>
       <c r="C62" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E62" s="3">
         <v>11</v>
@@ -2378,7 +2371,7 @@
         <v>253</v>
       </c>
       <c r="C63" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E63" s="3">
         <v>9</v>
@@ -2476,7 +2469,7 @@
         <v>225</v>
       </c>
       <c r="C70" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E70" s="3">
         <v>8</v>
@@ -2532,7 +2525,7 @@
         <v>230</v>
       </c>
       <c r="C74" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E74" s="3">
         <v>7</v>
@@ -2546,7 +2539,7 @@
         <v>231</v>
       </c>
       <c r="C75" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E75" s="3">
         <v>5</v>
@@ -2560,7 +2553,7 @@
         <v>221</v>
       </c>
       <c r="C76" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E76" s="3">
         <v>15</v>
@@ -2701,7 +2694,7 @@
         <v>246</v>
       </c>
       <c r="C85" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E85" s="3">
         <v>2</v>
@@ -2729,7 +2722,7 @@
         <v>253</v>
       </c>
       <c r="C87" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E87" s="3">
         <v>3</v>
@@ -2743,7 +2736,7 @@
         <v>254</v>
       </c>
       <c r="C88" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E88" s="3">
         <v>1</v>
@@ -2771,7 +2764,7 @@
         <v>221</v>
       </c>
       <c r="C90" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E90" s="3">
         <v>14</v>
@@ -2813,7 +2806,7 @@
         <v>225</v>
       </c>
       <c r="C93" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E93" s="3">
         <v>1</v>
@@ -2841,7 +2834,7 @@
         <v>219</v>
       </c>
       <c r="C95" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E95" s="3">
         <v>1</v>
@@ -2855,7 +2848,7 @@
         <v>231</v>
       </c>
       <c r="C96" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E96" s="3">
         <v>3</v>
@@ -2987,7 +2980,7 @@
         <v>253</v>
       </c>
       <c r="C105" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E105" s="3">
         <v>3</v>
@@ -3001,7 +2994,7 @@
         <v>221</v>
       </c>
       <c r="C106" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E106" s="3">
         <v>3</v>
@@ -3099,7 +3092,7 @@
         <v>229</v>
       </c>
       <c r="C113" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E113" s="3">
         <v>2</v>
@@ -3113,7 +3106,7 @@
         <v>232</v>
       </c>
       <c r="C114" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E114" s="3">
         <v>4</v>
@@ -3197,7 +3190,7 @@
         <v>221</v>
       </c>
       <c r="C120" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E120" s="3">
         <v>4</v>
@@ -3239,7 +3232,7 @@
         <v>215</v>
       </c>
       <c r="C123" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E123" s="3">
         <v>4</v>
@@ -3337,7 +3330,7 @@
         <v>229</v>
       </c>
       <c r="C130" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E130" s="3">
         <v>2</v>
@@ -3505,7 +3498,7 @@
         <v>215</v>
       </c>
       <c r="C142" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E142" s="3">
         <v>4</v>
@@ -3575,7 +3568,7 @@
         <v>229</v>
       </c>
       <c r="C147" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E147" s="3">
         <v>4</v>
@@ -3589,7 +3582,7 @@
         <v>230</v>
       </c>
       <c r="C148" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E148" s="3">
         <v>1</v>
@@ -3690,7 +3683,7 @@
         <v>221</v>
       </c>
       <c r="C155" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E155" s="3">
         <v>2</v>
@@ -3718,7 +3711,7 @@
         <v>215</v>
       </c>
       <c r="C157" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E157" s="3">
         <v>2</v>
@@ -3774,7 +3767,7 @@
         <v>229</v>
       </c>
       <c r="C161" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E161" s="3">
         <v>1</v>
@@ -3830,7 +3823,7 @@
         <v>246</v>
       </c>
       <c r="C165" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E165" s="3">
         <v>5</v>
@@ -3844,7 +3837,7 @@
         <v>221</v>
       </c>
       <c r="C166" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E166" s="3">
         <v>1</v>
@@ -3900,7 +3893,7 @@
         <v>229</v>
       </c>
       <c r="C170" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E170" s="3">
         <v>2</v>
@@ -3987,7 +3980,7 @@
         <v>246</v>
       </c>
       <c r="C176" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E176" s="3">
         <v>3</v>
@@ -4001,7 +3994,7 @@
         <v>215</v>
       </c>
       <c r="C177" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E177" s="3">
         <v>1</v>
@@ -4169,7 +4162,7 @@
         <v>235</v>
       </c>
       <c r="C189" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E189" s="3">
         <v>24</v>
@@ -4231,7 +4224,7 @@
         <v>246</v>
       </c>
       <c r="C193" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E193" s="3">
         <v>2</v>
@@ -4273,7 +4266,7 @@
         <v>250</v>
       </c>
       <c r="C196" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E196" s="3">
         <v>1</v>
@@ -4307,7 +4300,7 @@
         <v>2</v>
       </c>
       <c r="F198" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.35">
@@ -4332,7 +4325,7 @@
         <v>254</v>
       </c>
       <c r="C200" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E200" s="3">
         <v>1</v>
@@ -4388,7 +4381,7 @@
         <v>235</v>
       </c>
       <c r="C204" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E204" s="3">
         <v>9</v>
@@ -4590,7 +4583,7 @@
         <v>1</v>
       </c>
       <c r="F218" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.35">
@@ -4629,7 +4622,7 @@
         <v>221</v>
       </c>
       <c r="C221" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E221" s="3">
         <v>1</v>
@@ -4671,7 +4664,7 @@
         <v>235</v>
       </c>
       <c r="C224" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E224" s="3">
         <v>1</v>
@@ -4856,7 +4849,7 @@
         <v>246</v>
       </c>
       <c r="C237" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E237" s="3">
         <v>2</v>
@@ -4926,7 +4919,7 @@
         <v>250</v>
       </c>
       <c r="C242" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E242" s="3">
         <v>1</v>
@@ -4940,7 +4933,7 @@
         <v>253</v>
       </c>
       <c r="C243" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E243" s="3">
         <v>2</v>
@@ -4968,7 +4961,7 @@
         <v>254</v>
       </c>
       <c r="C245" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E245" s="3">
         <v>8</v>
@@ -5232,7 +5225,7 @@
         <v>246</v>
       </c>
       <c r="C263" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E263" s="3">
         <v>1</v>
@@ -5288,7 +5281,7 @@
         <v>249</v>
       </c>
       <c r="C267" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E267" s="3">
         <v>1</v>
@@ -5546,7 +5539,7 @@
         <v>246</v>
       </c>
       <c r="C285" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E285" s="3">
         <v>2</v>
@@ -5790,7 +5783,7 @@
         <v>259</v>
       </c>
       <c r="C302" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E302" s="3">
         <v>1</v>
@@ -5995,7 +5988,7 @@
         <v>221</v>
       </c>
       <c r="C316" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E316" s="3">
         <v>1</v>
@@ -7432,7 +7425,7 @@
         <v>219</v>
       </c>
       <c r="C415" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E415" s="3">
         <v>1</v>
@@ -7814,7 +7807,7 @@
         <v>262</v>
       </c>
       <c r="C441" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E441" s="3">
         <v>1</v>
@@ -7853,7 +7846,7 @@
         <v>38563</v>
       </c>
       <c r="B444" t="s">
-        <v>266</v>
+        <v>67</v>
       </c>
       <c r="C444" t="s">
         <v>68</v>
@@ -7867,7 +7860,7 @@
         <v>38563</v>
       </c>
       <c r="B445" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C445" t="s">
         <v>175</v>
@@ -7881,7 +7874,7 @@
         <v>38563</v>
       </c>
       <c r="B446" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C446" t="s">
         <v>173</v>
@@ -7895,7 +7888,7 @@
         <v>38563</v>
       </c>
       <c r="B447" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C447" t="s">
         <v>70</v>
@@ -7909,7 +7902,7 @@
         <v>38563</v>
       </c>
       <c r="B448" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C448" t="s">
         <v>74</v>
@@ -7923,7 +7916,7 @@
         <v>38563</v>
       </c>
       <c r="B449" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C449" t="s">
         <v>76</v>
@@ -7937,7 +7930,7 @@
         <v>38563</v>
       </c>
       <c r="B450" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C450" t="s">
         <v>82</v>
@@ -7951,7 +7944,7 @@
         <v>38563</v>
       </c>
       <c r="B451" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C451" t="s">
         <v>144</v>
@@ -7965,10 +7958,10 @@
         <v>38563</v>
       </c>
       <c r="B452" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C452" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E452" s="3">
         <v>1</v>
@@ -7979,7 +7972,7 @@
         <v>38563</v>
       </c>
       <c r="B453" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C453" t="s">
         <v>26</v>
@@ -7993,7 +7986,7 @@
         <v>38563</v>
       </c>
       <c r="B454" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C454" t="s">
         <v>12</v>
@@ -8007,7 +8000,7 @@
         <v>38563</v>
       </c>
       <c r="B455" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C455" t="s">
         <v>14</v>
@@ -8021,7 +8014,7 @@
         <v>38563</v>
       </c>
       <c r="B456" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C456" t="s">
         <v>16</v>
@@ -8035,7 +8028,7 @@
         <v>38563</v>
       </c>
       <c r="B457" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C457" t="s">
         <v>20</v>
@@ -8049,7 +8042,7 @@
         <v>38563</v>
       </c>
       <c r="B458" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C458" t="s">
         <v>24</v>
@@ -8063,7 +8056,7 @@
         <v>38563</v>
       </c>
       <c r="B459" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C459" t="s">
         <v>98</v>
@@ -8077,7 +8070,7 @@
         <v>38563</v>
       </c>
       <c r="B460" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C460" t="s">
         <v>28</v>
@@ -8091,7 +8084,7 @@
         <v>38563</v>
       </c>
       <c r="B461" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C461" t="s">
         <v>30</v>
@@ -8105,7 +8098,7 @@
         <v>38563</v>
       </c>
       <c r="B462" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C462" t="s">
         <v>104</v>
@@ -8119,7 +8112,7 @@
         <v>38563</v>
       </c>
       <c r="B463" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C463" t="s">
         <v>38</v>
@@ -8133,7 +8126,7 @@
         <v>38563</v>
       </c>
       <c r="B464" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C464" t="s">
         <v>110</v>
@@ -8147,7 +8140,7 @@
         <v>38563</v>
       </c>
       <c r="B465" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C465" t="s">
         <v>40</v>
@@ -8161,7 +8154,7 @@
         <v>38563</v>
       </c>
       <c r="B466" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C466" t="s">
         <v>44</v>
@@ -8175,7 +8168,7 @@
         <v>38563</v>
       </c>
       <c r="B467" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C467" t="s">
         <v>112</v>
@@ -8189,7 +8182,7 @@
         <v>38563</v>
       </c>
       <c r="B468" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C468" t="s">
         <v>48</v>
@@ -8203,7 +8196,7 @@
         <v>38563</v>
       </c>
       <c r="B469" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C469" t="s">
         <v>52</v>
@@ -8217,7 +8210,7 @@
         <v>38563</v>
       </c>
       <c r="B470" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C470" t="s">
         <v>158</v>
@@ -8259,10 +8252,10 @@
         <v>38563</v>
       </c>
       <c r="B473" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C473" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E473" s="3">
         <v>1</v>
@@ -8287,7 +8280,7 @@
         <v>38563</v>
       </c>
       <c r="B475" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C475" t="s">
         <v>141</v>
@@ -8301,10 +8294,10 @@
         <v>38563</v>
       </c>
       <c r="B476" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C476" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E476" s="3">
         <v>2</v>
@@ -8315,10 +8308,10 @@
         <v>38563</v>
       </c>
       <c r="B477" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C477" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E477" s="3">
         <v>2</v>
@@ -8427,7 +8420,7 @@
         <v>38941</v>
       </c>
       <c r="B485" t="s">
-        <v>266</v>
+        <v>67</v>
       </c>
       <c r="C485" t="s">
         <v>68</v>
@@ -8441,7 +8434,7 @@
         <v>38941</v>
       </c>
       <c r="B486" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C486" t="s">
         <v>187</v>
@@ -8455,7 +8448,7 @@
         <v>38941</v>
       </c>
       <c r="B487" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C487" t="s">
         <v>175</v>
@@ -8469,7 +8462,7 @@
         <v>38941</v>
       </c>
       <c r="B488" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C488" t="s">
         <v>70</v>
@@ -8483,7 +8476,7 @@
         <v>38941</v>
       </c>
       <c r="B489" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C489" t="s">
         <v>76</v>
@@ -8497,7 +8490,7 @@
         <v>38941</v>
       </c>
       <c r="B490" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C490" t="s">
         <v>78</v>
@@ -8511,7 +8504,7 @@
         <v>38941</v>
       </c>
       <c r="B491" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C491" t="s">
         <v>80</v>
@@ -8525,7 +8518,7 @@
         <v>38941</v>
       </c>
       <c r="B492" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C492" t="s">
         <v>82</v>
@@ -8539,7 +8532,7 @@
         <v>38941</v>
       </c>
       <c r="B493" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C493" t="s">
         <v>7</v>
@@ -8567,7 +8560,7 @@
         <v>38941</v>
       </c>
       <c r="B495" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C495" t="s">
         <v>12</v>
@@ -8581,7 +8574,7 @@
         <v>38941</v>
       </c>
       <c r="B496" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C496" t="s">
         <v>14</v>
@@ -8595,7 +8588,7 @@
         <v>38941</v>
       </c>
       <c r="B497" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C497" t="s">
         <v>16</v>
@@ -8609,7 +8602,7 @@
         <v>38941</v>
       </c>
       <c r="B498" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C498" t="s">
         <v>20</v>
@@ -8623,7 +8616,7 @@
         <v>38941</v>
       </c>
       <c r="B499" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C499" t="s">
         <v>24</v>
@@ -8637,7 +8630,7 @@
         <v>38941</v>
       </c>
       <c r="B500" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C500" t="s">
         <v>30</v>
@@ -8651,7 +8644,7 @@
         <v>38941</v>
       </c>
       <c r="B501" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C501" t="s">
         <v>32</v>
@@ -8665,7 +8658,7 @@
         <v>38941</v>
       </c>
       <c r="B502" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C502" t="s">
         <v>34</v>
@@ -8679,7 +8672,7 @@
         <v>38941</v>
       </c>
       <c r="B503" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C503" t="s">
         <v>38</v>
@@ -8693,7 +8686,7 @@
         <v>38941</v>
       </c>
       <c r="B504" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C504" t="s">
         <v>110</v>
@@ -8707,7 +8700,7 @@
         <v>38941</v>
       </c>
       <c r="B505" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C505" t="s">
         <v>46</v>
@@ -8721,7 +8714,7 @@
         <v>38941</v>
       </c>
       <c r="B506" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C506" t="s">
         <v>52</v>
@@ -8735,7 +8728,7 @@
         <v>38941</v>
       </c>
       <c r="B507" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C507" t="s">
         <v>158</v>
@@ -8763,7 +8756,7 @@
         <v>38941</v>
       </c>
       <c r="B509" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C509" t="s">
         <v>50</v>
@@ -8777,7 +8770,7 @@
         <v>38941</v>
       </c>
       <c r="B510" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C510" t="s">
         <v>121</v>
@@ -8878,7 +8871,7 @@
         <v>262</v>
       </c>
       <c r="C517" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E517" s="3">
         <v>14</v>
@@ -8931,7 +8924,7 @@
         <v>39299</v>
       </c>
       <c r="B521" t="s">
-        <v>266</v>
+        <v>67</v>
       </c>
       <c r="C521" t="s">
         <v>68</v>
@@ -8945,7 +8938,7 @@
         <v>39299</v>
       </c>
       <c r="B522" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C522" t="s">
         <v>187</v>
@@ -8959,7 +8952,7 @@
         <v>39299</v>
       </c>
       <c r="B523" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C523" t="s">
         <v>70</v>
@@ -8973,7 +8966,7 @@
         <v>39299</v>
       </c>
       <c r="B524" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C524" t="s">
         <v>72</v>
@@ -8987,7 +8980,7 @@
         <v>39299</v>
       </c>
       <c r="B525" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C525" t="s">
         <v>74</v>
@@ -9001,7 +8994,7 @@
         <v>39299</v>
       </c>
       <c r="B526" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C526" t="s">
         <v>76</v>
@@ -9015,7 +9008,7 @@
         <v>39299</v>
       </c>
       <c r="B527" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C527" t="s">
         <v>78</v>
@@ -9029,7 +9022,7 @@
         <v>39299</v>
       </c>
       <c r="B528" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C528" t="s">
         <v>80</v>
@@ -9043,7 +9036,7 @@
         <v>39299</v>
       </c>
       <c r="B529" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C529" t="s">
         <v>82</v>
@@ -9057,10 +9050,10 @@
         <v>39299</v>
       </c>
       <c r="B530" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C530" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E530" s="3">
         <v>2</v>
@@ -9071,7 +9064,7 @@
         <v>39299</v>
       </c>
       <c r="B531" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C531" t="s">
         <v>26</v>
@@ -9085,7 +9078,7 @@
         <v>39299</v>
       </c>
       <c r="B532" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C532" t="s">
         <v>7</v>
@@ -9099,7 +9092,7 @@
         <v>39299</v>
       </c>
       <c r="B533" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C533" t="s">
         <v>12</v>
@@ -9113,7 +9106,7 @@
         <v>39299</v>
       </c>
       <c r="B534" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C534" t="s">
         <v>14</v>
@@ -9127,7 +9120,7 @@
         <v>39299</v>
       </c>
       <c r="B535" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C535" t="s">
         <v>16</v>
@@ -9141,7 +9134,7 @@
         <v>39299</v>
       </c>
       <c r="B536" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C536" t="s">
         <v>18</v>
@@ -9155,7 +9148,7 @@
         <v>39299</v>
       </c>
       <c r="B537" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C537" t="s">
         <v>20</v>
@@ -9169,7 +9162,7 @@
         <v>39299</v>
       </c>
       <c r="B538" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C538" t="s">
         <v>24</v>
@@ -9183,7 +9176,7 @@
         <v>39299</v>
       </c>
       <c r="B539" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C539" t="s">
         <v>98</v>
@@ -9197,7 +9190,7 @@
         <v>39299</v>
       </c>
       <c r="B540" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C540" t="s">
         <v>28</v>
@@ -9211,7 +9204,7 @@
         <v>39299</v>
       </c>
       <c r="B541" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C541" t="s">
         <v>30</v>
@@ -9225,7 +9218,7 @@
         <v>39299</v>
       </c>
       <c r="B542" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C542" t="s">
         <v>32</v>
@@ -9239,7 +9232,7 @@
         <v>39299</v>
       </c>
       <c r="B543" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C543" t="s">
         <v>38</v>
@@ -9253,7 +9246,7 @@
         <v>39299</v>
       </c>
       <c r="B544" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C544" t="s">
         <v>110</v>
@@ -9267,7 +9260,7 @@
         <v>39299</v>
       </c>
       <c r="B545" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C545" t="s">
         <v>40</v>
@@ -9281,7 +9274,7 @@
         <v>39299</v>
       </c>
       <c r="B546" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C546" t="s">
         <v>42</v>
@@ -9295,7 +9288,7 @@
         <v>39299</v>
       </c>
       <c r="B547" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C547" t="s">
         <v>44</v>
@@ -9309,7 +9302,7 @@
         <v>39299</v>
       </c>
       <c r="B548" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C548" t="s">
         <v>46</v>
@@ -9323,7 +9316,7 @@
         <v>39299</v>
       </c>
       <c r="B549" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C549" t="s">
         <v>48</v>
@@ -9337,7 +9330,7 @@
         <v>39299</v>
       </c>
       <c r="B550" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C550" t="s">
         <v>158</v>
@@ -9393,7 +9386,7 @@
         <v>39299</v>
       </c>
       <c r="B554" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C554" t="s">
         <v>36</v>
@@ -9407,10 +9400,10 @@
         <v>39299</v>
       </c>
       <c r="B555" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C555" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E555" s="3">
         <v>1</v>
@@ -9421,7 +9414,7 @@
         <v>39299</v>
       </c>
       <c r="B556" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C556" t="s">
         <v>50</v>
@@ -9435,7 +9428,7 @@
         <v>39299</v>
       </c>
       <c r="B557" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C557" t="s">
         <v>52</v>
@@ -9449,7 +9442,7 @@
         <v>39299</v>
       </c>
       <c r="B558" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C558" t="s">
         <v>175</v>
@@ -9508,7 +9501,7 @@
         <v>262</v>
       </c>
       <c r="C562" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E562" s="3">
         <v>8</v>
@@ -9561,7 +9554,7 @@
         <v>39669</v>
       </c>
       <c r="B566" t="s">
-        <v>266</v>
+        <v>67</v>
       </c>
       <c r="C566" t="s">
         <v>68</v>
@@ -9575,7 +9568,7 @@
         <v>39669</v>
       </c>
       <c r="B567" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C567" t="s">
         <v>70</v>
@@ -9589,7 +9582,7 @@
         <v>39669</v>
       </c>
       <c r="B568" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C568" t="s">
         <v>72</v>
@@ -9603,7 +9596,7 @@
         <v>39669</v>
       </c>
       <c r="B569" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C569" t="s">
         <v>76</v>
@@ -9617,7 +9610,7 @@
         <v>39669</v>
       </c>
       <c r="B570" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C570" t="s">
         <v>78</v>
@@ -9631,7 +9624,7 @@
         <v>39669</v>
       </c>
       <c r="B571" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C571" t="s">
         <v>80</v>
@@ -9645,7 +9638,7 @@
         <v>39669</v>
       </c>
       <c r="B572" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C572" t="s">
         <v>82</v>
@@ -9659,7 +9652,7 @@
         <v>39669</v>
       </c>
       <c r="B573" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C573" t="s">
         <v>144</v>
@@ -9673,7 +9666,7 @@
         <v>39669</v>
       </c>
       <c r="B574" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C574" t="s">
         <v>38</v>
@@ -9687,7 +9680,7 @@
         <v>39669</v>
       </c>
       <c r="B575" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C575" t="s">
         <v>40</v>
@@ -9701,7 +9694,7 @@
         <v>39669</v>
       </c>
       <c r="B576" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C576" t="s">
         <v>46</v>
@@ -9715,7 +9708,7 @@
         <v>39669</v>
       </c>
       <c r="B577" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C577" t="s">
         <v>48</v>
@@ -9729,7 +9722,7 @@
         <v>39669</v>
       </c>
       <c r="B578" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C578" t="s">
         <v>52</v>
@@ -9743,7 +9736,7 @@
         <v>39669</v>
       </c>
       <c r="B579" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C579" t="s">
         <v>50</v>
@@ -9757,7 +9750,7 @@
         <v>39669</v>
       </c>
       <c r="B580" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C580" t="s">
         <v>175</v>
@@ -9785,13 +9778,13 @@
         <v>39669</v>
       </c>
       <c r="B582" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E582" s="3">
         <v>12</v>
       </c>
       <c r="F582" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="583" spans="1:6" x14ac:dyDescent="0.35">
@@ -9799,13 +9792,13 @@
         <v>39669</v>
       </c>
       <c r="B583" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E583" s="3">
         <v>9</v>
       </c>
       <c r="F583" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="584" spans="1:6" x14ac:dyDescent="0.35">
@@ -9900,7 +9893,7 @@
         <v>262</v>
       </c>
       <c r="C590" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E590" s="3">
         <v>5</v>
@@ -9953,7 +9946,7 @@
         <v>40026</v>
       </c>
       <c r="B594" t="s">
-        <v>266</v>
+        <v>67</v>
       </c>
       <c r="C594" t="s">
         <v>68</v>
@@ -9967,7 +9960,7 @@
         <v>40026</v>
       </c>
       <c r="B595" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C595" t="s">
         <v>70</v>
@@ -9981,7 +9974,7 @@
         <v>40026</v>
       </c>
       <c r="B596" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C596" t="s">
         <v>72</v>
@@ -9995,7 +9988,7 @@
         <v>40026</v>
       </c>
       <c r="B597" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C597" t="s">
         <v>76</v>
@@ -10009,7 +10002,7 @@
         <v>40026</v>
       </c>
       <c r="B598" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C598" t="s">
         <v>78</v>
@@ -10023,7 +10016,7 @@
         <v>40026</v>
       </c>
       <c r="B599" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C599" t="s">
         <v>80</v>
@@ -10037,7 +10030,7 @@
         <v>40026</v>
       </c>
       <c r="B600" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C600" t="s">
         <v>82</v>
@@ -10051,7 +10044,7 @@
         <v>40026</v>
       </c>
       <c r="B601" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C601" t="s">
         <v>144</v>
@@ -10065,7 +10058,7 @@
         <v>40026</v>
       </c>
       <c r="B602" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C602" t="s">
         <v>26</v>
@@ -10079,7 +10072,7 @@
         <v>40026</v>
       </c>
       <c r="B603" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C603" t="s">
         <v>7</v>
@@ -10107,7 +10100,7 @@
         <v>40026</v>
       </c>
       <c r="B605" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C605" t="s">
         <v>12</v>
@@ -10121,7 +10114,7 @@
         <v>40026</v>
       </c>
       <c r="B606" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C606" t="s">
         <v>14</v>
@@ -10135,7 +10128,7 @@
         <v>40026</v>
       </c>
       <c r="B607" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C607" t="s">
         <v>16</v>
@@ -10149,7 +10142,7 @@
         <v>40026</v>
       </c>
       <c r="B608" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C608" t="s">
         <v>18</v>
@@ -10163,7 +10156,7 @@
         <v>40026</v>
       </c>
       <c r="B609" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C609" t="s">
         <v>20</v>
@@ -10177,7 +10170,7 @@
         <v>40026</v>
       </c>
       <c r="B610" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C610" t="s">
         <v>24</v>
@@ -10191,7 +10184,7 @@
         <v>40026</v>
       </c>
       <c r="B611" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C611" t="s">
         <v>98</v>
@@ -10205,7 +10198,7 @@
         <v>40026</v>
       </c>
       <c r="B612" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C612" t="s">
         <v>28</v>
@@ -10219,7 +10212,7 @@
         <v>40026</v>
       </c>
       <c r="B613" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C613" t="s">
         <v>30</v>
@@ -10233,7 +10226,7 @@
         <v>40026</v>
       </c>
       <c r="B614" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C614" t="s">
         <v>32</v>
@@ -10247,7 +10240,7 @@
         <v>40026</v>
       </c>
       <c r="B615" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C615" t="s">
         <v>34</v>
@@ -10261,7 +10254,7 @@
         <v>40026</v>
       </c>
       <c r="B616" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C616" t="s">
         <v>38</v>
@@ -10275,7 +10268,7 @@
         <v>40026</v>
       </c>
       <c r="B617" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C617" t="s">
         <v>110</v>
@@ -10289,7 +10282,7 @@
         <v>40026</v>
       </c>
       <c r="B618" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C618" t="s">
         <v>40</v>
@@ -10303,7 +10296,7 @@
         <v>40026</v>
       </c>
       <c r="B619" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C619" t="s">
         <v>42</v>
@@ -10317,7 +10310,7 @@
         <v>40026</v>
       </c>
       <c r="B620" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C620" t="s">
         <v>44</v>
@@ -10331,7 +10324,7 @@
         <v>40026</v>
       </c>
       <c r="B621" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C621" t="s">
         <v>46</v>
@@ -10345,7 +10338,7 @@
         <v>40026</v>
       </c>
       <c r="B622" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C622" t="s">
         <v>48</v>
@@ -10359,7 +10352,7 @@
         <v>40026</v>
       </c>
       <c r="B623" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C623" t="s">
         <v>52</v>
@@ -10373,7 +10366,7 @@
         <v>40026</v>
       </c>
       <c r="B624" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C624" t="s">
         <v>189</v>
@@ -10488,7 +10481,7 @@
         <v>262</v>
       </c>
       <c r="C632" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E632" s="3">
         <v>19</v>
@@ -10541,7 +10534,7 @@
         <v>40391</v>
       </c>
       <c r="B636" t="s">
-        <v>266</v>
+        <v>67</v>
       </c>
       <c r="C636" t="s">
         <v>68</v>
@@ -10555,7 +10548,7 @@
         <v>40391</v>
       </c>
       <c r="B637" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C637" t="s">
         <v>187</v>
@@ -10569,7 +10562,7 @@
         <v>40391</v>
       </c>
       <c r="B638" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C638" t="s">
         <v>173</v>
@@ -10583,7 +10576,7 @@
         <v>40391</v>
       </c>
       <c r="B639" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C639" t="s">
         <v>70</v>
@@ -10597,7 +10590,7 @@
         <v>40391</v>
       </c>
       <c r="B640" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C640" t="s">
         <v>72</v>
@@ -10611,7 +10604,7 @@
         <v>40391</v>
       </c>
       <c r="B641" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C641" t="s">
         <v>74</v>
@@ -10625,7 +10618,7 @@
         <v>40391</v>
       </c>
       <c r="B642" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C642" t="s">
         <v>76</v>
@@ -10639,7 +10632,7 @@
         <v>40391</v>
       </c>
       <c r="B643" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C643" t="s">
         <v>78</v>
@@ -10653,7 +10646,7 @@
         <v>40391</v>
       </c>
       <c r="B644" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C644" t="s">
         <v>80</v>
@@ -10667,7 +10660,7 @@
         <v>40391</v>
       </c>
       <c r="B645" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C645" t="s">
         <v>82</v>
@@ -10681,7 +10674,7 @@
         <v>40391</v>
       </c>
       <c r="B646" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C646" t="s">
         <v>144</v>
@@ -10695,10 +10688,10 @@
         <v>40391</v>
       </c>
       <c r="B647" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C647" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E647" s="3">
         <v>1</v>
@@ -10709,7 +10702,7 @@
         <v>40391</v>
       </c>
       <c r="B648" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C648" t="s">
         <v>26</v>
@@ -10810,7 +10803,7 @@
         <v>262</v>
       </c>
       <c r="C655" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E655" s="3">
         <v>8</v>
@@ -10849,7 +10842,7 @@
         <v>40761</v>
       </c>
       <c r="B658" t="s">
-        <v>266</v>
+        <v>67</v>
       </c>
       <c r="C658" t="s">
         <v>68</v>
@@ -10863,7 +10856,7 @@
         <v>40761</v>
       </c>
       <c r="B659" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C659" t="s">
         <v>187</v>
@@ -10877,7 +10870,7 @@
         <v>40761</v>
       </c>
       <c r="B660" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C660" t="s">
         <v>70</v>
@@ -10891,7 +10884,7 @@
         <v>40761</v>
       </c>
       <c r="B661" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C661" t="s">
         <v>72</v>
@@ -10905,7 +10898,7 @@
         <v>40761</v>
       </c>
       <c r="B662" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C662" t="s">
         <v>74</v>
@@ -10919,7 +10912,7 @@
         <v>40761</v>
       </c>
       <c r="B663" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C663" t="s">
         <v>76</v>
@@ -10933,7 +10926,7 @@
         <v>40761</v>
       </c>
       <c r="B664" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C664" t="s">
         <v>78</v>
@@ -10947,7 +10940,7 @@
         <v>40761</v>
       </c>
       <c r="B665" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C665" t="s">
         <v>80</v>
@@ -10961,7 +10954,7 @@
         <v>40761</v>
       </c>
       <c r="B666" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C666" t="s">
         <v>82</v>
@@ -10975,7 +10968,7 @@
         <v>40761</v>
       </c>
       <c r="B667" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C667" t="s">
         <v>26</v>
@@ -10989,7 +10982,7 @@
         <v>40761</v>
       </c>
       <c r="B668" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C668" t="s">
         <v>7</v>
@@ -11017,7 +11010,7 @@
         <v>40761</v>
       </c>
       <c r="B670" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C670" t="s">
         <v>12</v>
@@ -11031,7 +11024,7 @@
         <v>40761</v>
       </c>
       <c r="B671" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C671" t="s">
         <v>14</v>
@@ -11045,7 +11038,7 @@
         <v>40761</v>
       </c>
       <c r="B672" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C672" t="s">
         <v>165</v>
@@ -11059,7 +11052,7 @@
         <v>40761</v>
       </c>
       <c r="B673" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C673" t="s">
         <v>16</v>
@@ -11073,7 +11066,7 @@
         <v>40761</v>
       </c>
       <c r="B674" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C674" t="s">
         <v>20</v>
@@ -11087,7 +11080,7 @@
         <v>40761</v>
       </c>
       <c r="B675" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C675" t="s">
         <v>24</v>
@@ -11101,7 +11094,7 @@
         <v>40761</v>
       </c>
       <c r="B676" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C676" t="s">
         <v>98</v>
@@ -11115,7 +11108,7 @@
         <v>40761</v>
       </c>
       <c r="B677" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C677" t="s">
         <v>28</v>
@@ -11129,7 +11122,7 @@
         <v>40761</v>
       </c>
       <c r="B678" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C678" t="s">
         <v>30</v>
@@ -11143,7 +11136,7 @@
         <v>40761</v>
       </c>
       <c r="B679" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C679" t="s">
         <v>34</v>
@@ -11157,7 +11150,7 @@
         <v>40761</v>
       </c>
       <c r="B680" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C680" t="s">
         <v>38</v>
@@ -11171,7 +11164,7 @@
         <v>40761</v>
       </c>
       <c r="B681" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C681" t="s">
         <v>110</v>
@@ -11185,7 +11178,7 @@
         <v>40761</v>
       </c>
       <c r="B682" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C682" t="s">
         <v>40</v>
@@ -11199,7 +11192,7 @@
         <v>40761</v>
       </c>
       <c r="B683" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C683" t="s">
         <v>44</v>
@@ -11213,7 +11206,7 @@
         <v>40761</v>
       </c>
       <c r="B684" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C684" t="s">
         <v>46</v>
@@ -11227,7 +11220,7 @@
         <v>40761</v>
       </c>
       <c r="B685" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C685" t="s">
         <v>48</v>
@@ -11241,7 +11234,7 @@
         <v>40761</v>
       </c>
       <c r="B686" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C686" t="s">
         <v>52</v>
@@ -11255,7 +11248,7 @@
         <v>40761</v>
       </c>
       <c r="B687" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C687" t="s">
         <v>189</v>
@@ -11311,7 +11304,7 @@
         <v>40761</v>
       </c>
       <c r="B691" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C691" t="s">
         <v>36</v>
@@ -11325,7 +11318,7 @@
         <v>40761</v>
       </c>
       <c r="B692" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C692" t="s">
         <v>191</v>
@@ -11339,7 +11332,7 @@
         <v>40761</v>
       </c>
       <c r="B693" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C693" t="s">
         <v>141</v>
@@ -11353,10 +11346,10 @@
         <v>40761</v>
       </c>
       <c r="B694" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C694" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E694" s="3">
         <v>2</v>
@@ -11367,7 +11360,7 @@
         <v>40761</v>
       </c>
       <c r="B695" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C695" t="s">
         <v>121</v>

</xml_diff>